<commit_message>
Repeat test raise a bug, v0p5_LTE
</commit_message>
<xml_diff>
--- a/MotorMotionControlModule/Protocol_NeodAnderjon.xlsx
+++ b/MotorMotionControlModule/Protocol_NeodAnderjon.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+  <si>
+    <r>
       <t>EmbeddedBreakerCore</t>
     </r>
     <r>
@@ -82,12 +76,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">0A </t>
     </r>
     <r>
@@ -105,12 +93,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">0B </t>
     </r>
     <r>
@@ -125,12 +107,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -145,12 +121,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -165,12 +135,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">0C </t>
     </r>
     <r>
@@ -223,12 +187,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">0E </t>
     </r>
     <r>
@@ -281,12 +239,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">0F </t>
     </r>
     <r>
@@ -301,12 +253,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -321,12 +267,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -341,12 +281,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t>MotorMotionController</t>
     </r>
     <r>
@@ -550,12 +484,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">1A </t>
     </r>
     <r>
@@ -570,12 +498,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -590,12 +512,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -630,12 +546,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -650,12 +560,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -690,12 +594,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -710,12 +608,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -730,12 +622,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -750,12 +636,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -770,12 +650,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">02 </t>
     </r>
     <r>
@@ -790,12 +664,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">03 </t>
     </r>
     <r>
@@ -837,12 +705,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">04 </t>
     </r>
     <r>
@@ -857,12 +719,20 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
+      <t xml:space="preserve">05 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>正反转重复性测试</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1B </t>
     </r>
     <r>
@@ -1122,12 +992,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">00 </t>
     </r>
     <r>
@@ -1142,12 +1006,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -1171,7 +1029,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1189,7 +1047,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1200,53 +1058,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1262,7 +1075,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1270,7 +1090,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1278,14 +1120,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1308,7 +1143,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1316,15 +1175,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1352,187 +1203,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,7 +1401,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1558,8 +1409,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1575,6 +1441,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1604,190 +1494,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2143,10 +1994,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD20"/>
+  <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.3"/>
@@ -2176,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:18">
+    <row r="2" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2187,7 +2038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" s="2" customFormat="1" spans="1:18">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2243,7 +2094,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:18">
+    <row r="4" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2254,7 +2105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:18">
+    <row r="5" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2268,12 +2119,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="3:3">
+    <row r="6" s="2" customFormat="1" ht="15.75" spans="3:3">
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:18">
+    <row r="7" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2287,7 +2138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:18">
+    <row r="8" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2301,7 +2152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:18">
+    <row r="9" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2315,7 +2166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="3:3">
+    <row r="10" s="2" customFormat="1" ht="15.75" spans="3:3">
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2325,7 +2176,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:18">
+    <row r="12" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2360,7 +2211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:18">
+    <row r="13" s="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2395,7 +2246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="3:15">
+    <row r="14" s="2" customFormat="1" ht="15.75" spans="3:15">
       <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
@@ -2409,80 +2260,68 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="3:3">
+    <row r="15" s="2" customFormat="1" ht="15.75" spans="3:3">
       <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="3:3">
+    <row r="16" s="2" customFormat="1" ht="15.75" spans="3:3">
       <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="3:3">
+    <row r="17" s="2" customFormat="1" ht="15.75" spans="3:3">
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:18">
-      <c r="A18" s="2" t="s">
+    <row r="18" s="2" customFormat="1" ht="15.75" spans="3:3">
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" ht="15.75" spans="1:18">
+      <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="P19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="3:15">
-      <c r="C19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="3:15">
+    <row r="20" s="2" customFormat="1" ht="15.75" spans="3:15">
       <c r="C20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2497,6 +2336,23 @@
       </c>
       <c r="O20" s="2" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" ht="15.75" spans="3:15">
+      <c r="C21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>